<commit_message>
add script for computing training battery number
</commit_message>
<xml_diff>
--- a/results/fig5_CALB_data.xlsx
+++ b/results/fig5_CALB_data.xlsx
@@ -475,10 +475,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3641864017949341</v>
+        <v>0.4300749247744064</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2373917889769497</v>
+        <v>0.255263897198904</v>
       </c>
       <c r="D2" t="n">
         <v>0.2315269619844571</v>
@@ -498,10 +498,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.201327246774304</v>
+        <v>0.1717761142610414</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0984210455185878</v>
+        <v>0.1034552040444705</v>
       </c>
       <c r="D3" t="n">
         <v>0.2373196759681131</v>
@@ -521,10 +521,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1890830438849314</v>
+        <v>0.1568383829265867</v>
       </c>
       <c r="C4" t="n">
-        <v>0.07088668695257037</v>
+        <v>0.0785677708644221</v>
       </c>
       <c r="D4" t="n">
         <v>0.2345706395466745</v>
@@ -544,10 +544,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1822864759571562</v>
+        <v>0.143112926340585</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05138274043134183</v>
+        <v>0.06981572904065483</v>
       </c>
       <c r="D5" t="n">
         <v>0.195949701905294</v>
@@ -567,10 +567,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1792047902598639</v>
+        <v>0.1360098636777746</v>
       </c>
       <c r="C6" t="n">
-        <v>0.05024676945876723</v>
+        <v>0.06862109809018667</v>
       </c>
       <c r="D6" t="n">
         <v>0.1960195213670506</v>
@@ -590,10 +590,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1653275151398896</v>
+        <v>0.1288367523129157</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06397585829127787</v>
+        <v>0.06794019481209386</v>
       </c>
       <c r="D7" t="n">
         <v>0.1948695738597064</v>
@@ -613,10 +613,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1516544818952965</v>
+        <v>0.1300230604221381</v>
       </c>
       <c r="C8" t="n">
-        <v>0.06480667228648614</v>
+        <v>0.05858999541637945</v>
       </c>
       <c r="D8" t="n">
         <v>0.1826419410394281</v>
@@ -636,10 +636,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.136286908241597</v>
+        <v>0.1320408868390709</v>
       </c>
       <c r="C9" t="n">
-        <v>0.05821487533006058</v>
+        <v>0.05431879241211775</v>
       </c>
       <c r="D9" t="n">
         <v>0.1682348395608183</v>
@@ -659,10 +659,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1516238785438791</v>
+        <v>0.1523044183757928</v>
       </c>
       <c r="C10" t="n">
-        <v>0.05457308110960565</v>
+        <v>0.05521574770574234</v>
       </c>
       <c r="D10" t="n">
         <v>0.1717802372976267</v>
@@ -682,10 +682,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1484399108675609</v>
+        <v>0.1463449460930414</v>
       </c>
       <c r="C11" t="n">
-        <v>0.05308528611445684</v>
+        <v>0.05120057766040832</v>
       </c>
       <c r="D11" t="n">
         <v>0.1752026855986243</v>
@@ -705,10 +705,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1548932905635172</v>
+        <v>0.1460247566892164</v>
       </c>
       <c r="C12" t="n">
-        <v>0.05307934027626598</v>
+        <v>0.04718687877090438</v>
       </c>
       <c r="D12" t="n">
         <v>0.1691753254677734</v>
@@ -728,10 +728,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1481501617544776</v>
+        <v>0.1358286691973563</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0464517074826874</v>
+        <v>0.03857065126435414</v>
       </c>
       <c r="D13" t="n">
         <v>0.1750909715436084</v>
@@ -751,10 +751,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1432245015606333</v>
+        <v>0.1267705750477363</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0440266701021739</v>
+        <v>0.03870927753243644</v>
       </c>
       <c r="D14" t="n">
         <v>0.1768861718426409</v>
@@ -774,10 +774,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.1172799459962649</v>
+        <v>0.1023315904416462</v>
       </c>
       <c r="C15" t="n">
-        <v>0.04038783972751926</v>
+        <v>0.03384841093270213</v>
       </c>
       <c r="D15" t="n">
         <v>0.16777261274487</v>
@@ -797,10 +797,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1221935519379257</v>
+        <v>0.1024561660031886</v>
       </c>
       <c r="C16" t="n">
-        <v>0.04866335810388057</v>
+        <v>0.04808580090662353</v>
       </c>
       <c r="D16" t="n">
         <v>0.1642386650729496</v>
@@ -820,10 +820,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1235940783037071</v>
+        <v>0.1040885145340021</v>
       </c>
       <c r="C17" t="n">
-        <v>0.04307148347682558</v>
+        <v>0.043369363391465</v>
       </c>
       <c r="D17" t="n">
         <v>0.1690466213931482</v>
@@ -843,10 +843,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1293339635508688</v>
+        <v>0.1034794990760372</v>
       </c>
       <c r="C18" t="n">
-        <v>0.04579478498650104</v>
+        <v>0.04360870467898132</v>
       </c>
       <c r="D18" t="n">
         <v>0.1614657007935461</v>
@@ -866,10 +866,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1330407809510354</v>
+        <v>0.1092418721902008</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0456452962714932</v>
+        <v>0.045010318447292</v>
       </c>
       <c r="D19" t="n">
         <v>0.1628952780435554</v>
@@ -889,10 +889,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1062629946196469</v>
+        <v>0.08977033304375535</v>
       </c>
       <c r="C20" t="n">
-        <v>0.02574273386393538</v>
+        <v>0.02073594441626765</v>
       </c>
       <c r="D20" t="n">
         <v>0.1568013667333734</v>
@@ -912,10 +912,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1023149172151376</v>
+        <v>0.08952148221757839</v>
       </c>
       <c r="C21" t="n">
-        <v>0.02379911999625004</v>
+        <v>0.006898011531314086</v>
       </c>
       <c r="D21" t="n">
         <v>0.1484830347743092</v>
@@ -935,10 +935,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.09968726945523158</v>
+        <v>0.09378119339549112</v>
       </c>
       <c r="C22" t="n">
-        <v>0.02258953300533042</v>
+        <v>0.01919091528435141</v>
       </c>
       <c r="D22" t="n">
         <v>0.1567829702442118</v>
@@ -958,10 +958,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>0.09015434935329698</v>
+        <v>0.08083484083274091</v>
       </c>
       <c r="C23" t="n">
-        <v>0.02192439034498764</v>
+        <v>0.01408039575873342</v>
       </c>
       <c r="D23" t="n">
         <v>0.1556329349591743</v>
@@ -981,10 +981,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0.09517856498422621</v>
+        <v>0.08527391782931266</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01004863811458881</v>
+        <v>0.01274175302691839</v>
       </c>
       <c r="D24" t="n">
         <v>0.1518691265595893</v>
@@ -1004,10 +1004,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>0.0930956584531374</v>
+        <v>0.08419729153349453</v>
       </c>
       <c r="C25" t="n">
-        <v>0.00987940336005955</v>
+        <v>0.02201480042206815</v>
       </c>
       <c r="D25" t="n">
         <v>0.1478284097177874</v>
@@ -1027,10 +1027,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>0.08713499489196323</v>
+        <v>0.08033402235818908</v>
       </c>
       <c r="C26" t="n">
-        <v>0.008944805304165459</v>
+        <v>0.01856249441289346</v>
       </c>
       <c r="D26" t="n">
         <v>0.1425769131811877</v>
@@ -1050,10 +1050,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>0.1109038902498051</v>
+        <v>0.0976790225935643</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01667298171270869</v>
+        <v>0.01678053484984869</v>
       </c>
       <c r="D27" t="n">
         <v>0.1451492970225357</v>
@@ -1073,10 +1073,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>0.09692685514877862</v>
+        <v>0.1012760710287428</v>
       </c>
       <c r="C28" t="n">
-        <v>0.02990529881507027</v>
+        <v>0.02805606497256286</v>
       </c>
       <c r="D28" t="n">
         <v>0.1535585101450521</v>
@@ -1096,10 +1096,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>0.09356873870349165</v>
+        <v>0.0967897493707864</v>
       </c>
       <c r="C29" t="n">
-        <v>0.02418831246834548</v>
+        <v>0.02326512514366445</v>
       </c>
       <c r="D29" t="n">
         <v>0.1529528148301384</v>
@@ -1119,10 +1119,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>0.09823405746760978</v>
+        <v>0.09365118996493151</v>
       </c>
       <c r="C30" t="n">
-        <v>0.02115193929432953</v>
+        <v>0.02401221839941894</v>
       </c>
       <c r="D30" t="n">
         <v>0.1478953615815355</v>
@@ -1142,10 +1142,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>0.09072954407487481</v>
+        <v>0.08142991621251149</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01453388145085124</v>
+        <v>0.02606644353908011</v>
       </c>
       <c r="D31" t="n">
         <v>0.1475014585842147</v>
@@ -1165,10 +1165,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>0.09897466501939838</v>
+        <v>0.08746635085144581</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0150747363622014</v>
+        <v>0.03063501413566459</v>
       </c>
       <c r="D32" t="n">
         <v>0.1374285554794414</v>
@@ -1188,10 +1188,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>0.09495721265568779</v>
+        <v>0.08409066837899161</v>
       </c>
       <c r="C33" t="n">
-        <v>0.00553989037377076</v>
+        <v>0.01901175078183716</v>
       </c>
       <c r="D33" t="n">
         <v>0.1348204572387598</v>
@@ -1211,10 +1211,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0918259590427109</v>
+        <v>0.08853714259238217</v>
       </c>
       <c r="C34" t="n">
-        <v>0.002086066292351284</v>
+        <v>0.002713611280464382</v>
       </c>
       <c r="D34" t="n">
         <v>0.1327189617363498</v>
@@ -1234,10 +1234,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>0.08615031394833363</v>
+        <v>0.08210766012758869</v>
       </c>
       <c r="C35" t="n">
-        <v>0.01127584360674551</v>
+        <v>0.005589199376317727</v>
       </c>
       <c r="D35" t="n">
         <v>0.1319008071667958</v>
@@ -1257,10 +1257,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>0.0873191379580298</v>
+        <v>0.08456707463309182</v>
       </c>
       <c r="C36" t="n">
-        <v>0.01032761641741184</v>
+        <v>0.006527936863498254</v>
       </c>
       <c r="D36" t="n">
         <v>0.1320586503236196</v>
@@ -1280,10 +1280,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>0.08277643238270825</v>
+        <v>0.0758248630695374</v>
       </c>
       <c r="C37" t="n">
-        <v>0.009316370380939994</v>
+        <v>0.009636910980224862</v>
       </c>
       <c r="D37" t="n">
         <v>0.125039575797144</v>
@@ -1303,10 +1303,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>0.07524674827893303</v>
+        <v>0.06753055003311664</v>
       </c>
       <c r="C38" t="n">
-        <v>0.002760019337971714</v>
+        <v>0.008621111649060079</v>
       </c>
       <c r="D38" t="n">
         <v>0.1281105154548828</v>
@@ -1326,10 +1326,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>0.07858999460389325</v>
+        <v>0.07543217142111232</v>
       </c>
       <c r="C39" t="n">
-        <v>0.01863444954567562</v>
+        <v>0.02197400681826609</v>
       </c>
       <c r="D39" t="n">
         <v>0.1278448494574096</v>
@@ -1349,10 +1349,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>0.0822869445598453</v>
+        <v>0.08191633176986363</v>
       </c>
       <c r="C40" t="n">
-        <v>0.03155626481932234</v>
+        <v>0.03187847694313574</v>
       </c>
       <c r="D40" t="n">
         <v>0.1276442592490877</v>
@@ -1372,10 +1372,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>0.104201463175276</v>
+        <v>0.1003640184005662</v>
       </c>
       <c r="C41" t="n">
-        <v>0.03680877065261699</v>
+        <v>0.0398575428851586</v>
       </c>
       <c r="D41" t="n">
         <v>0.1246906614583568</v>
@@ -1395,10 +1395,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>0.1107330794292666</v>
+        <v>0.1011829614231063</v>
       </c>
       <c r="C42" t="n">
-        <v>0.04187672141318173</v>
+        <v>0.04859758772460227</v>
       </c>
       <c r="D42" t="n">
         <v>0.1196900569768609</v>
@@ -1418,10 +1418,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>0.1000581905599674</v>
+        <v>0.09243801983044524</v>
       </c>
       <c r="C43" t="n">
-        <v>0.02309992472696037</v>
+        <v>0.02883799668211805</v>
       </c>
       <c r="D43" t="n">
         <v>0.1194074907818394</v>
@@ -1441,10 +1441,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0786637237880476</v>
+        <v>0.07308990712034526</v>
       </c>
       <c r="C44" t="n">
-        <v>0.008425710653026868</v>
+        <v>0.001747746818155209</v>
       </c>
       <c r="D44" t="n">
         <v>0.1166855225251293</v>
@@ -1464,10 +1464,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>0.0803719657814591</v>
+        <v>0.08694570433132769</v>
       </c>
       <c r="C45" t="n">
-        <v>0.004415941098178677</v>
+        <v>0.01242159548961644</v>
       </c>
       <c r="D45" t="n">
         <v>0.1179516053009321</v>
@@ -1487,10 +1487,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>0.07869143277599684</v>
+        <v>0.09369786697778433</v>
       </c>
       <c r="C46" t="n">
-        <v>0.002609254491086632</v>
+        <v>0.01892580649906158</v>
       </c>
       <c r="D46" t="n">
         <v>0.1159898027556692</v>
@@ -1510,10 +1510,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>0.09879068549103227</v>
+        <v>0.1140258115508374</v>
       </c>
       <c r="C47" t="n">
-        <v>0.0174289540856015</v>
+        <v>0.02053542208712198</v>
       </c>
       <c r="D47" t="n">
         <v>0.1082091453832009</v>
@@ -1533,10 +1533,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>0.09539315176819795</v>
+        <v>0.1041828367511729</v>
       </c>
       <c r="C48" t="n">
-        <v>0.03021590011148067</v>
+        <v>0.02998586886126967</v>
       </c>
       <c r="D48" t="n">
         <v>0.1058903520629497</v>
@@ -1556,10 +1556,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>0.09472027880513634</v>
+        <v>0.08929911241700071</v>
       </c>
       <c r="C49" t="n">
-        <v>0.02526096594326433</v>
+        <v>0.02571540885011694</v>
       </c>
       <c r="D49" t="n">
         <v>0.1057828443944285</v>
@@ -1579,10 +1579,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>0.09428493530057365</v>
+        <v>0.07918697344873739</v>
       </c>
       <c r="C50" t="n">
-        <v>0.01553345166843247</v>
+        <v>0.01344500578522714</v>
       </c>
       <c r="D50" t="n">
         <v>0.1038926508346621</v>
@@ -1602,10 +1602,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>0.08091200743150025</v>
+        <v>0.07285939929506219</v>
       </c>
       <c r="C51" t="n">
-        <v>0.006662364569557147</v>
+        <v>0.007749596513067742</v>
       </c>
       <c r="D51" t="n">
         <v>0.1064587874409914</v>
@@ -1625,10 +1625,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>0.08433301202052074</v>
+        <v>0.07694193496065201</v>
       </c>
       <c r="C52" t="n">
-        <v>0.006667202879169922</v>
+        <v>0.01530853837800051</v>
       </c>
       <c r="D52" t="n">
         <v>0.1064823945738308</v>
@@ -1648,10 +1648,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>0.08722731648855896</v>
+        <v>0.08402552901929239</v>
       </c>
       <c r="C53" t="n">
-        <v>0.008233524078631062</v>
+        <v>0.01239550783891361</v>
       </c>
       <c r="D53" t="n">
         <v>0.1068066391774598</v>
@@ -1671,10 +1671,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>0.07342220588698047</v>
+        <v>0.07236124748366234</v>
       </c>
       <c r="C54" t="n">
-        <v>0.01325657463082085</v>
+        <v>0.01361867811866617</v>
       </c>
       <c r="D54" t="n">
         <v>0.1108169931935387</v>
@@ -1694,10 +1694,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>0.07686272011584332</v>
+        <v>0.06487624109429171</v>
       </c>
       <c r="C55" t="n">
-        <v>0.004702537005197622</v>
+        <v>0.01817194813500781</v>
       </c>
       <c r="D55" t="n">
         <v>0.1130229495629244</v>
@@ -1717,10 +1717,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>0.09483229268429703</v>
+        <v>0.07108843157304107</v>
       </c>
       <c r="C56" t="n">
-        <v>0.0207290033182962</v>
+        <v>0.03688174464749321</v>
       </c>
       <c r="D56" t="n">
         <v>0.1150962675361349</v>
@@ -1740,10 +1740,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>0.07931733383666141</v>
+        <v>0.05604620257888263</v>
       </c>
       <c r="C57" t="n">
-        <v>0.0221208336083758</v>
+        <v>0.02445121738746085</v>
       </c>
       <c r="D57" t="n">
         <v>0.1138606449978757</v>
@@ -1763,10 +1763,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0645644271878273</v>
+        <v>0.05465933902835964</v>
       </c>
       <c r="C58" t="n">
-        <v>0.01084979277949695</v>
+        <v>0.003524604781005429</v>
       </c>
       <c r="D58" t="n">
         <v>0.1122460073504223</v>
@@ -1786,10 +1786,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>0.06394786060389428</v>
+        <v>0.06887843117171989</v>
       </c>
       <c r="C59" t="n">
-        <v>0.00639254317221884</v>
+        <v>0.01153254538421886</v>
       </c>
       <c r="D59" t="n">
         <v>0.1089437242296245</v>
@@ -1809,10 +1809,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0697405723764787</v>
+        <v>0.08275545553463291</v>
       </c>
       <c r="C60" t="n">
-        <v>0.009741014256456968</v>
+        <v>0.008710825525360807</v>
       </c>
       <c r="D60" t="n">
         <v>0.1132118909656108</v>
@@ -1832,10 +1832,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>0.09175877777624068</v>
+        <v>0.1058896240267333</v>
       </c>
       <c r="C61" t="n">
-        <v>0.0190740373928092</v>
+        <v>0.007518502716552698</v>
       </c>
       <c r="D61" t="n">
         <v>0.1103436084166093</v>
@@ -1855,10 +1855,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>0.1011870546245353</v>
+        <v>0.1039204439251719</v>
       </c>
       <c r="C62" t="n">
-        <v>0.0183788410202791</v>
+        <v>0.01515402755015257</v>
       </c>
       <c r="D62" t="n">
         <v>0.1096342025844017</v>
@@ -1878,10 +1878,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>0.09467793809999613</v>
+        <v>0.08985976623380644</v>
       </c>
       <c r="C63" t="n">
-        <v>0.005677959915599533</v>
+        <v>0.01180012707065736</v>
       </c>
       <c r="D63" t="n">
         <v>0.1122938029582049</v>
@@ -1901,10 +1901,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>0.08119108965415558</v>
+        <v>0.07168277671263855</v>
       </c>
       <c r="C64" t="n">
-        <v>0.002947788045243625</v>
+        <v>0.01050342193777969</v>
       </c>
       <c r="D64" t="n">
         <v>0.1109342655765339</v>
@@ -1924,10 +1924,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>0.07474501465996883</v>
+        <v>0.06435102592286089</v>
       </c>
       <c r="C65" t="n">
-        <v>0.01433698426088122</v>
+        <v>0.0007713366319274972</v>
       </c>
       <c r="D65" t="n">
         <v>0.1125233534575695</v>
@@ -1947,10 +1947,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>0.08320907613725143</v>
+        <v>0.06807405551394941</v>
       </c>
       <c r="C66" t="n">
-        <v>0.02397735139399066</v>
+        <v>0.01737818878692008</v>
       </c>
       <c r="D66" t="n">
         <v>0.1155722961950308</v>
@@ -1970,10 +1970,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>0.08560759043468051</v>
+        <v>0.07016506546092947</v>
       </c>
       <c r="C67" t="n">
-        <v>0.01843549700773044</v>
+        <v>0.01367123173715661</v>
       </c>
       <c r="D67" t="n">
         <v>0.1111023482671599</v>
@@ -1993,10 +1993,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>0.09248119807781596</v>
+        <v>0.0782191123888477</v>
       </c>
       <c r="C68" t="n">
-        <v>0.01545641227195919</v>
+        <v>0.02007297753441954</v>
       </c>
       <c r="D68" t="n">
         <v>0.1116202265507961</v>
@@ -2016,10 +2016,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>0.08350417279411548</v>
+        <v>0.0754102305978452</v>
       </c>
       <c r="C69" t="n">
-        <v>0.01048789510344268</v>
+        <v>0.01454738886054256</v>
       </c>
       <c r="D69" t="n">
         <v>0.1145074187548979</v>
@@ -2039,10 +2039,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>0.07009464666135783</v>
+        <v>0.06647596225623131</v>
       </c>
       <c r="C70" t="n">
-        <v>0.008904590352699051</v>
+        <v>0.007527435002320327</v>
       </c>
       <c r="D70" t="n">
         <v>0.1177539793257127</v>
@@ -2062,10 +2062,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>0.06533894748539271</v>
+        <v>0.07370373318125384</v>
       </c>
       <c r="C71" t="n">
-        <v>0.01020935174300811</v>
+        <v>0.01260270761866227</v>
       </c>
       <c r="D71" t="n">
         <v>0.1187536995186071</v>
@@ -2085,10 +2085,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>0.06933387607141545</v>
+        <v>0.08117393938247863</v>
       </c>
       <c r="C72" t="n">
-        <v>0.01555555086617821</v>
+        <v>0.01679563941586899</v>
       </c>
       <c r="D72" t="n">
         <v>0.1137755661527644</v>
@@ -2108,10 +2108,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>0.07289372695238339</v>
+        <v>0.08299209712771165</v>
       </c>
       <c r="C73" t="n">
-        <v>0.01287515471519768</v>
+        <v>0.004514448361414266</v>
       </c>
       <c r="D73" t="n">
         <v>0.1161675733999921</v>
@@ -2131,10 +2131,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>0.07967859140732465</v>
+        <v>0.08293004840133987</v>
       </c>
       <c r="C74" t="n">
-        <v>0.01500131851067881</v>
+        <v>0.01197553815312427</v>
       </c>
       <c r="D74" t="n">
         <v>0.1140250513016755</v>
@@ -2154,10 +2154,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>0.06893381434637146</v>
+        <v>0.06780223723861284</v>
       </c>
       <c r="C75" t="n">
-        <v>0.01537709541116422</v>
+        <v>0.01457733697646168</v>
       </c>
       <c r="D75" t="n">
         <v>0.1142711905007527</v>
@@ -2177,10 +2177,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>0.07080372457687978</v>
+        <v>0.07000216531176549</v>
       </c>
       <c r="C76" t="n">
-        <v>0.01030424127799166</v>
+        <v>0.009236712301453349</v>
       </c>
       <c r="D76" t="n">
         <v>0.114427312368508</v>
@@ -2200,10 +2200,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>0.07474047996079759</v>
+        <v>0.07513741639506734</v>
       </c>
       <c r="C77" t="n">
-        <v>0.0106781942043606</v>
+        <v>0.01123491105147523</v>
       </c>
       <c r="D77" t="n">
         <v>0.1139026730219059</v>
@@ -2223,10 +2223,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>0.08126132916471014</v>
+        <v>0.08276784074971909</v>
       </c>
       <c r="C78" t="n">
-        <v>0.008153571596967</v>
+        <v>0.009724087772840624</v>
       </c>
       <c r="D78" t="n">
         <v>0.1162605223766887</v>
@@ -2246,10 +2246,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>0.07897844766563926</v>
+        <v>0.0769896537116443</v>
       </c>
       <c r="C79" t="n">
-        <v>0.01412545968187535</v>
+        <v>0.01132306657880019</v>
       </c>
       <c r="D79" t="n">
         <v>0.1182184871032234</v>
@@ -2269,10 +2269,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>0.06944992469125175</v>
+        <v>0.06606113973699955</v>
       </c>
       <c r="C80" t="n">
-        <v>0.01016238294113886</v>
+        <v>0.005441413778288919</v>
       </c>
       <c r="D80" t="n">
         <v>0.1223080256314032</v>
@@ -2292,10 +2292,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>0.06461673917947593</v>
+        <v>0.05865250347158121</v>
       </c>
       <c r="C81" t="n">
-        <v>0.007900885805647776</v>
+        <v>0.002978682526953628</v>
       </c>
       <c r="D81" t="n">
         <v>0.1240711091235513</v>
@@ -2315,10 +2315,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>0.06531402534862052</v>
+        <v>0.05744863650733654</v>
       </c>
       <c r="C82" t="n">
-        <v>0.009655483763820926</v>
+        <v>0.004852373330513417</v>
       </c>
       <c r="D82" t="n">
         <v>0.1250525515387599</v>
@@ -2338,10 +2338,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>0.06432572952506785</v>
+        <v>0.06622203886548773</v>
       </c>
       <c r="C83" t="n">
-        <v>0.004901027777011997</v>
+        <v>0.003437022046452075</v>
       </c>
       <c r="D83" t="n">
         <v>0.1279468042270303</v>
@@ -2361,10 +2361,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>0.06732825685737918</v>
+        <v>0.07447137464029184</v>
       </c>
       <c r="C84" t="n">
-        <v>0.006432463892941906</v>
+        <v>0.01341068042717724</v>
       </c>
       <c r="D84" t="n">
         <v>0.1279787653826953</v>
@@ -2384,10 +2384,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>0.07106416907099138</v>
+        <v>0.07882521884546649</v>
       </c>
       <c r="C85" t="n">
-        <v>0.01244654351983137</v>
+        <v>0.0234220429280523</v>
       </c>
       <c r="D85" t="n">
         <v>0.1275550115125526</v>
@@ -2407,10 +2407,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>0.07579315999459389</v>
+        <v>0.08157391182166629</v>
       </c>
       <c r="C86" t="n">
-        <v>0.01385926871876359</v>
+        <v>0.02145378611037379</v>
       </c>
       <c r="D86" t="n">
         <v>0.13029955898689</v>
@@ -2430,10 +2430,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>0.08044956058403743</v>
+        <v>0.07304613314339761</v>
       </c>
       <c r="C87" t="n">
-        <v>0.02396661245283253</v>
+        <v>0.01556504989395628</v>
       </c>
       <c r="D87" t="n">
         <v>0.131136399264919</v>
@@ -2453,10 +2453,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>0.07220862027923784</v>
+        <v>0.05991946628498342</v>
       </c>
       <c r="C88" t="n">
-        <v>0.02202493510123597</v>
+        <v>0.007801761709659998</v>
       </c>
       <c r="D88" t="n">
         <v>0.1315313371134813</v>
@@ -2476,10 +2476,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>0.07054925137062759</v>
+        <v>0.05999019788891292</v>
       </c>
       <c r="C89" t="n">
-        <v>0.01670711860822428</v>
+        <v>0.004883127808673013</v>
       </c>
       <c r="D89" t="n">
         <v>0.1346879246701988</v>
@@ -2499,10 +2499,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>0.07483636855722067</v>
+        <v>0.06374764641765181</v>
       </c>
       <c r="C90" t="n">
-        <v>0.01375387055071167</v>
+        <v>0.01065654578423371</v>
       </c>
       <c r="D90" t="n">
         <v>0.1332517863720364</v>
@@ -2522,10 +2522,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>0.07507009081284455</v>
+        <v>0.06874377762530136</v>
       </c>
       <c r="C91" t="n">
-        <v>0.01092396173772381</v>
+        <v>0.01093009901957999</v>
       </c>
       <c r="D91" t="n">
         <v>0.1335496908453785</v>
@@ -2545,10 +2545,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>0.0870077792515261</v>
+        <v>0.07582843247653197</v>
       </c>
       <c r="C92" t="n">
-        <v>0.01279848957760218</v>
+        <v>0.01721911889800938</v>
       </c>
       <c r="D92" t="n">
         <v>0.1354700008045439</v>
@@ -2568,10 +2568,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>0.07914299695391651</v>
+        <v>0.06705480886828546</v>
       </c>
       <c r="C93" t="n">
-        <v>0.01930194345758144</v>
+        <v>0.02425849108481481</v>
       </c>
       <c r="D93" t="n">
         <v>0.1353303806259686</v>
@@ -2591,10 +2591,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>0.0780922035245996</v>
+        <v>0.06828583778611307</v>
       </c>
       <c r="C94" t="n">
-        <v>0.0242122376463151</v>
+        <v>0.02730132483899393</v>
       </c>
       <c r="D94" t="n">
         <v>0.1360904616295363</v>
@@ -2614,10 +2614,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>0.07730184199171157</v>
+        <v>0.07278713359664916</v>
       </c>
       <c r="C95" t="n">
-        <v>0.01031406272240014</v>
+        <v>0.01323560431098768</v>
       </c>
       <c r="D95" t="n">
         <v>0.136595488523571</v>
@@ -2637,10 +2637,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>0.06753740103270164</v>
+        <v>0.07160894397714614</v>
       </c>
       <c r="C96" t="n">
-        <v>0.004950132948035783</v>
+        <v>0.007710898749870223</v>
       </c>
       <c r="D96" t="n">
         <v>0.137862384330988</v>
@@ -2660,10 +2660,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>0.06822106284503902</v>
+        <v>0.07523794044613664</v>
       </c>
       <c r="C97" t="n">
-        <v>0.01134209499089894</v>
+        <v>0.0154795348372804</v>
       </c>
       <c r="D97" t="n">
         <v>0.1396821422291354</v>
@@ -2683,10 +2683,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>0.06935152144647543</v>
+        <v>0.0683451299359254</v>
       </c>
       <c r="C98" t="n">
-        <v>0.01038339380210254</v>
+        <v>0.009380302500482414</v>
       </c>
       <c r="D98" t="n">
         <v>0.1401734601232492</v>
@@ -2706,10 +2706,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>0.07281274631067132</v>
+        <v>0.05986633555157698</v>
       </c>
       <c r="C99" t="n">
-        <v>0.01287729308939971</v>
+        <v>0.007686175920898666</v>
       </c>
       <c r="D99" t="n">
         <v>0.137604582919526</v>
@@ -2729,10 +2729,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>0.0806464935866648</v>
+        <v>0.05924353447614746</v>
       </c>
       <c r="C100" t="n">
-        <v>0.01043141184119614</v>
+        <v>0.01983992916609123</v>
       </c>
       <c r="D100" t="n">
         <v>0.1334431518798016</v>
@@ -2752,10 +2752,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>0.1006521629252587</v>
+        <v>0.08565057024599994</v>
       </c>
       <c r="C101" t="n">
-        <v>0.009865392059571538</v>
+        <v>0.03013640926435517</v>
       </c>
       <c r="D101" t="n">
         <v>0.1258187561931292</v>

</xml_diff>